<commit_message>
chore: manual redeploy after retailers.xlsx update
</commit_message>
<xml_diff>
--- a/data/retailers.xlsx
+++ b/data/retailers.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jbailey\certis_agroute_app\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{37F84A02-3E54-461A-9C66-1F16D72F63EC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{696035C2-AF05-41A7-A78B-A8558F3CA640}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="291" yWindow="1740" windowWidth="19200" windowHeight="8391" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1900" yWindow="1900" windowWidth="14400" windowHeight="7270" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Combined" sheetId="1" r:id="rId1"/>
@@ -8305,7 +8305,7 @@
   <dimension ref="A1:I991"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="I1" sqref="I1"/>
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="26.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -8440,7 +8440,7 @@
         <v>20</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="F5" s="2" t="s">
         <v>12</v>
@@ -37219,6 +37219,15 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <lcf76f155ced4ddcb4097134ff3c332f xmlns="7cecf09e-87d6-4345-a370-97524ef8da64">
@@ -37226,15 +37235,6 @@
     </lcf76f155ced4ddcb4097134ff3c332f>
   </documentManagement>
 </p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -37256,6 +37256,14 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{10CF58AA-00EF-4BDF-A97C-BB1A0168CFB8}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9BF1610B-6E8D-417B-A267-064FFADDBB14}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
@@ -37263,12 +37271,4 @@
     <ds:schemaRef ds:uri="7cecf09e-87d6-4345-a370-97524ef8da64"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{10CF58AA-00EF-4BDF-A97C-BB1A0168CFB8}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
🚀 Deploy latest CertisMap fixes
</commit_message>
<xml_diff>
--- a/data/retailers.xlsx
+++ b/data/retailers.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jbailey\certis_agroute_app\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23AC8CD1-37C3-4164-B7FB-4B31D81162A7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{79CB057A-981E-4415-B060-6CE54C677F1A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1900" yWindow="1900" windowWidth="14400" windowHeight="7270" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Combined" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7988" uniqueCount="2638">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8324" uniqueCount="2743">
   <si>
     <t>Retailer</t>
   </si>
@@ -7934,6 +7934,321 @@
   </si>
   <si>
     <t>Suppliers</t>
+  </si>
+  <si>
+    <t>Frenchman Valley Coop</t>
+  </si>
+  <si>
+    <t>Benkelman – Convenience Store, Service Station, Energy</t>
+  </si>
+  <si>
+    <t>33797 Hwy 34</t>
+  </si>
+  <si>
+    <t>Benkelman</t>
+  </si>
+  <si>
+    <t>Benkelman – Grain Elevator</t>
+  </si>
+  <si>
+    <t>303 W Railroad</t>
+  </si>
+  <si>
+    <t>Burns – Grain Elevator</t>
+  </si>
+  <si>
+    <t>420 Coop Rd</t>
+  </si>
+  <si>
+    <t>Burns</t>
+  </si>
+  <si>
+    <t>WY</t>
+  </si>
+  <si>
+    <t>Chappell – Agronomy</t>
+  </si>
+  <si>
+    <t>16515 County Road 14</t>
+  </si>
+  <si>
+    <t>Chappell</t>
+  </si>
+  <si>
+    <t>Chappell – Energy</t>
+  </si>
+  <si>
+    <t>582 2nd St</t>
+  </si>
+  <si>
+    <t>Chappell – Grain Elevator, Feed</t>
+  </si>
+  <si>
+    <t>Culbertson – East Grain Elevator</t>
+  </si>
+  <si>
+    <t>168 Clarkston</t>
+  </si>
+  <si>
+    <t>Culbertson</t>
+  </si>
+  <si>
+    <t>Culbertson – Shuttle Loader</t>
+  </si>
+  <si>
+    <t>37252 US Hwy 34</t>
+  </si>
+  <si>
+    <t>Dalton – Energy/Cardtrol Pumps</t>
+  </si>
+  <si>
+    <t>602 Broad St</t>
+  </si>
+  <si>
+    <t>Dalton</t>
+  </si>
+  <si>
+    <t>Dix – Grain Elevator</t>
+  </si>
+  <si>
+    <t>110 Spruce St</t>
+  </si>
+  <si>
+    <t>Dix</t>
+  </si>
+  <si>
+    <t>Enders – Grain Elevator</t>
+  </si>
+  <si>
+    <t>Pioneer and 1st Street</t>
+  </si>
+  <si>
+    <t>Enders</t>
+  </si>
+  <si>
+    <t>Grant – Agronomy</t>
+  </si>
+  <si>
+    <t>32945 Nebraska 23</t>
+  </si>
+  <si>
+    <t>Grant</t>
+  </si>
+  <si>
+    <t>Grant – East Elevator</t>
+  </si>
+  <si>
+    <t>75985 Rd 329</t>
+  </si>
+  <si>
+    <t>Grant – Fertilizer</t>
+  </si>
+  <si>
+    <t>32870 Rd 759 ¾</t>
+  </si>
+  <si>
+    <t>Imperial – Aerial</t>
+  </si>
+  <si>
+    <t>100 Hwy 61</t>
+  </si>
+  <si>
+    <t>Imperial</t>
+  </si>
+  <si>
+    <t>Imperial – Agronomy / 24‑HR Diesel Pumps</t>
+  </si>
+  <si>
+    <t>101 Douglas Street</t>
+  </si>
+  <si>
+    <t>Imperial – Corporate HQ / Main Office</t>
+  </si>
+  <si>
+    <t>202 Broadway Street (PO Box 578)</t>
+  </si>
+  <si>
+    <t>Imperial – Feed</t>
+  </si>
+  <si>
+    <t>143 Broadway</t>
+  </si>
+  <si>
+    <t>Feed</t>
+  </si>
+  <si>
+    <t>Imperial – Grain Elevators</t>
+  </si>
+  <si>
+    <t>Imperial – Service Station</t>
+  </si>
+  <si>
+    <t>103 W 3rd St</t>
+  </si>
+  <si>
+    <t>Imperial – T‑Junction</t>
+  </si>
+  <si>
+    <t>Hwy 6 &amp; 61</t>
+  </si>
+  <si>
+    <t>Kimball – Cardtrol Pumps</t>
+  </si>
+  <si>
+    <t>1105 S Chestnut St</t>
+  </si>
+  <si>
+    <t>Kimball – Feed</t>
+  </si>
+  <si>
+    <t>Kimball – Grain Elevator</t>
+  </si>
+  <si>
+    <t>3980 W Main</t>
+  </si>
+  <si>
+    <t>Lodgepole – Grain Elevator</t>
+  </si>
+  <si>
+    <t>607 Sheldon</t>
+  </si>
+  <si>
+    <t>Lodgepole</t>
+  </si>
+  <si>
+    <t>Lodgepole – Convenience Store / Cardtrol Pumps</t>
+  </si>
+  <si>
+    <t>607 Sheldon St</t>
+  </si>
+  <si>
+    <t>McCook – Agronomy</t>
+  </si>
+  <si>
+    <t>203 Karrer St</t>
+  </si>
+  <si>
+    <t>McCook</t>
+  </si>
+  <si>
+    <t>McCook – Convenience Store / Energy</t>
+  </si>
+  <si>
+    <t>206 East B St</t>
+  </si>
+  <si>
+    <t>McCook – Feed</t>
+  </si>
+  <si>
+    <t>301 W A St</t>
+  </si>
+  <si>
+    <t>McCook – Grain Elevator</t>
+  </si>
+  <si>
+    <t>102 E 3rd St</t>
+  </si>
+  <si>
+    <t>McCook – Xpress 24‑Hr Fueling</t>
+  </si>
+  <si>
+    <t>South Hwy 83</t>
+  </si>
+  <si>
+    <t>Oshkosh – Grain Elevator</t>
+  </si>
+  <si>
+    <t>205 U.S. 26</t>
+  </si>
+  <si>
+    <t>Oshkosh</t>
+  </si>
+  <si>
+    <t>Palisade – Grain Elevator</t>
+  </si>
+  <si>
+    <t>102 N Dean St</t>
+  </si>
+  <si>
+    <t>Palisade</t>
+  </si>
+  <si>
+    <t>Pine Bluffs – Agronomy</t>
+  </si>
+  <si>
+    <t>100 North Main</t>
+  </si>
+  <si>
+    <t>Pine Bluffs</t>
+  </si>
+  <si>
+    <t>Pine Bluffs – Energy/Cardtrol Pumps</t>
+  </si>
+  <si>
+    <t>102 Walnut Street</t>
+  </si>
+  <si>
+    <t>Pine Bluffs – Grain Elevator</t>
+  </si>
+  <si>
+    <t>605 W US Hwy 30</t>
+  </si>
+  <si>
+    <t>Potter – Energy / Cardtrol Pumps</t>
+  </si>
+  <si>
+    <t>3040 Link 17B</t>
+  </si>
+  <si>
+    <t>Potter</t>
+  </si>
+  <si>
+    <t>Sidney – Agronomy</t>
+  </si>
+  <si>
+    <t>303 Illinois St</t>
+  </si>
+  <si>
+    <t>Sidney</t>
+  </si>
+  <si>
+    <t>Sidney – Energy / Cardtrol Pumps</t>
+  </si>
+  <si>
+    <t>1402 Illinois St</t>
+  </si>
+  <si>
+    <t>Venango – Grain Elevator</t>
+  </si>
+  <si>
+    <t>104 East Hwy 23</t>
+  </si>
+  <si>
+    <t>Venango</t>
+  </si>
+  <si>
+    <t>Wauneta – Grain Elevator</t>
+  </si>
+  <si>
+    <t>102 N Tecumseh St</t>
+  </si>
+  <si>
+    <t>Wauneta</t>
+  </si>
+  <si>
+    <t>Wheatland – Energy / Cardtrol Pumps</t>
+  </si>
+  <si>
+    <t>305 16th St</t>
+  </si>
+  <si>
+    <t>Wheatland</t>
+  </si>
+  <si>
+    <t>Frenchman Valley Coop - NE WY</t>
+  </si>
+  <si>
+    <t>Wilbur-Ellis, Helena, Nutrien</t>
   </si>
 </sst>
 </file>
@@ -8299,13 +8614,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I991"/>
+  <dimension ref="A1:I1033"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+    <sheetView tabSelected="1" topLeftCell="D1030" workbookViewId="0">
+      <selection activeCell="J1030" sqref="J1030"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="26.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="35.7265625" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
@@ -37036,6 +37354,1224 @@
       </c>
       <c r="I991" s="2" t="s">
         <v>14</v>
+      </c>
+    </row>
+    <row r="992" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A992" s="2" t="s">
+        <v>2741</v>
+      </c>
+      <c r="B992" s="2" t="s">
+        <v>2638</v>
+      </c>
+      <c r="C992" s="2" t="s">
+        <v>2639</v>
+      </c>
+      <c r="D992" s="2" t="s">
+        <v>2640</v>
+      </c>
+      <c r="E992" s="2" t="s">
+        <v>2641</v>
+      </c>
+      <c r="F992" s="2" t="s">
+        <v>520</v>
+      </c>
+      <c r="G992" s="2">
+        <v>69021</v>
+      </c>
+      <c r="H992" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="I992" s="2" t="s">
+        <v>2742</v>
+      </c>
+    </row>
+    <row r="993" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A993" s="2" t="s">
+        <v>2741</v>
+      </c>
+      <c r="B993" s="2" t="s">
+        <v>2638</v>
+      </c>
+      <c r="C993" s="2" t="s">
+        <v>2642</v>
+      </c>
+      <c r="D993" s="2" t="s">
+        <v>2643</v>
+      </c>
+      <c r="E993" s="2" t="s">
+        <v>2641</v>
+      </c>
+      <c r="F993" s="2" t="s">
+        <v>520</v>
+      </c>
+      <c r="G993" s="2">
+        <v>69021</v>
+      </c>
+      <c r="H993" s="2" t="s">
+        <v>225</v>
+      </c>
+      <c r="I993" s="2" t="s">
+        <v>2742</v>
+      </c>
+    </row>
+    <row r="994" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A994" s="2" t="s">
+        <v>2741</v>
+      </c>
+      <c r="B994" s="2" t="s">
+        <v>2638</v>
+      </c>
+      <c r="C994" s="2" t="s">
+        <v>2644</v>
+      </c>
+      <c r="D994" s="2" t="s">
+        <v>2645</v>
+      </c>
+      <c r="E994" s="2" t="s">
+        <v>2646</v>
+      </c>
+      <c r="F994" s="2" t="s">
+        <v>2647</v>
+      </c>
+      <c r="G994" s="2">
+        <v>82053</v>
+      </c>
+      <c r="H994" s="2" t="s">
+        <v>225</v>
+      </c>
+      <c r="I994" s="2" t="s">
+        <v>2742</v>
+      </c>
+    </row>
+    <row r="995" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A995" s="2" t="s">
+        <v>2741</v>
+      </c>
+      <c r="B995" s="2" t="s">
+        <v>2638</v>
+      </c>
+      <c r="C995" s="2" t="s">
+        <v>2648</v>
+      </c>
+      <c r="D995" s="2" t="s">
+        <v>2649</v>
+      </c>
+      <c r="E995" s="2" t="s">
+        <v>2650</v>
+      </c>
+      <c r="F995" s="2" t="s">
+        <v>520</v>
+      </c>
+      <c r="G995" s="2">
+        <v>69129</v>
+      </c>
+      <c r="H995" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="I995" s="2" t="s">
+        <v>2742</v>
+      </c>
+    </row>
+    <row r="996" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A996" s="2" t="s">
+        <v>2741</v>
+      </c>
+      <c r="B996" s="2" t="s">
+        <v>2638</v>
+      </c>
+      <c r="C996" s="2" t="s">
+        <v>2651</v>
+      </c>
+      <c r="D996" s="2" t="s">
+        <v>2652</v>
+      </c>
+      <c r="E996" s="2" t="s">
+        <v>2650</v>
+      </c>
+      <c r="F996" s="2" t="s">
+        <v>520</v>
+      </c>
+      <c r="G996" s="2">
+        <v>69129</v>
+      </c>
+      <c r="H996" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="I996" s="2" t="s">
+        <v>2742</v>
+      </c>
+    </row>
+    <row r="997" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A997" s="2" t="s">
+        <v>2741</v>
+      </c>
+      <c r="B997" s="2" t="s">
+        <v>2638</v>
+      </c>
+      <c r="C997" s="2" t="s">
+        <v>2653</v>
+      </c>
+      <c r="D997" s="2" t="s">
+        <v>2649</v>
+      </c>
+      <c r="E997" s="2" t="s">
+        <v>2650</v>
+      </c>
+      <c r="F997" s="2" t="s">
+        <v>520</v>
+      </c>
+      <c r="G997" s="2">
+        <v>69129</v>
+      </c>
+      <c r="H997" s="2" t="s">
+        <v>1646</v>
+      </c>
+      <c r="I997" s="2" t="s">
+        <v>2742</v>
+      </c>
+    </row>
+    <row r="998" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A998" s="2" t="s">
+        <v>2741</v>
+      </c>
+      <c r="B998" s="2" t="s">
+        <v>2638</v>
+      </c>
+      <c r="C998" s="2" t="s">
+        <v>2654</v>
+      </c>
+      <c r="D998" s="2" t="s">
+        <v>2655</v>
+      </c>
+      <c r="E998" s="2" t="s">
+        <v>2656</v>
+      </c>
+      <c r="F998" s="2" t="s">
+        <v>520</v>
+      </c>
+      <c r="G998" s="2">
+        <v>69024</v>
+      </c>
+      <c r="H998" s="2" t="s">
+        <v>225</v>
+      </c>
+      <c r="I998" s="2" t="s">
+        <v>2742</v>
+      </c>
+    </row>
+    <row r="999" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A999" s="2" t="s">
+        <v>2741</v>
+      </c>
+      <c r="B999" s="2" t="s">
+        <v>2638</v>
+      </c>
+      <c r="C999" s="2" t="s">
+        <v>2657</v>
+      </c>
+      <c r="D999" s="2" t="s">
+        <v>2658</v>
+      </c>
+      <c r="E999" s="2" t="s">
+        <v>2656</v>
+      </c>
+      <c r="F999" s="2" t="s">
+        <v>520</v>
+      </c>
+      <c r="G999" s="2">
+        <v>69024</v>
+      </c>
+      <c r="H999" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="I999" s="2" t="s">
+        <v>2742</v>
+      </c>
+    </row>
+    <row r="1000" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A1000" s="2" t="s">
+        <v>2741</v>
+      </c>
+      <c r="B1000" s="2" t="s">
+        <v>2638</v>
+      </c>
+      <c r="C1000" s="2" t="s">
+        <v>2659</v>
+      </c>
+      <c r="D1000" s="2" t="s">
+        <v>2660</v>
+      </c>
+      <c r="E1000" s="2" t="s">
+        <v>2661</v>
+      </c>
+      <c r="F1000" s="2" t="s">
+        <v>520</v>
+      </c>
+      <c r="G1000" s="2">
+        <v>69131</v>
+      </c>
+      <c r="H1000" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="I1000" s="2" t="s">
+        <v>2742</v>
+      </c>
+    </row>
+    <row r="1001" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A1001" s="2" t="s">
+        <v>2741</v>
+      </c>
+      <c r="B1001" s="2" t="s">
+        <v>2638</v>
+      </c>
+      <c r="C1001" s="2" t="s">
+        <v>2662</v>
+      </c>
+      <c r="D1001" s="2" t="s">
+        <v>2663</v>
+      </c>
+      <c r="E1001" s="2" t="s">
+        <v>2664</v>
+      </c>
+      <c r="F1001" s="2" t="s">
+        <v>520</v>
+      </c>
+      <c r="G1001" s="2">
+        <v>69133</v>
+      </c>
+      <c r="H1001" s="2" t="s">
+        <v>225</v>
+      </c>
+      <c r="I1001" s="2" t="s">
+        <v>2742</v>
+      </c>
+    </row>
+    <row r="1002" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A1002" s="2" t="s">
+        <v>2741</v>
+      </c>
+      <c r="B1002" s="2" t="s">
+        <v>2638</v>
+      </c>
+      <c r="C1002" s="2" t="s">
+        <v>2665</v>
+      </c>
+      <c r="D1002" s="2" t="s">
+        <v>2666</v>
+      </c>
+      <c r="E1002" s="2" t="s">
+        <v>2667</v>
+      </c>
+      <c r="F1002" s="2" t="s">
+        <v>520</v>
+      </c>
+      <c r="G1002" s="2">
+        <v>69027</v>
+      </c>
+      <c r="H1002" s="2" t="s">
+        <v>225</v>
+      </c>
+      <c r="I1002" s="2" t="s">
+        <v>2742</v>
+      </c>
+    </row>
+    <row r="1003" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A1003" s="2" t="s">
+        <v>2741</v>
+      </c>
+      <c r="B1003" s="2" t="s">
+        <v>2638</v>
+      </c>
+      <c r="C1003" s="2" t="s">
+        <v>2668</v>
+      </c>
+      <c r="D1003" s="2" t="s">
+        <v>2669</v>
+      </c>
+      <c r="E1003" s="2" t="s">
+        <v>2670</v>
+      </c>
+      <c r="F1003" s="2" t="s">
+        <v>520</v>
+      </c>
+      <c r="G1003" s="2">
+        <v>69140</v>
+      </c>
+      <c r="H1003" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="I1003" s="2" t="s">
+        <v>2742</v>
+      </c>
+    </row>
+    <row r="1004" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A1004" s="2" t="s">
+        <v>2741</v>
+      </c>
+      <c r="B1004" s="2" t="s">
+        <v>2638</v>
+      </c>
+      <c r="C1004" s="2" t="s">
+        <v>2671</v>
+      </c>
+      <c r="D1004" s="2" t="s">
+        <v>2672</v>
+      </c>
+      <c r="E1004" s="2" t="s">
+        <v>2670</v>
+      </c>
+      <c r="F1004" s="2" t="s">
+        <v>520</v>
+      </c>
+      <c r="G1004" s="2">
+        <v>69140</v>
+      </c>
+      <c r="H1004" s="2" t="s">
+        <v>225</v>
+      </c>
+      <c r="I1004" s="2" t="s">
+        <v>2742</v>
+      </c>
+    </row>
+    <row r="1005" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A1005" s="2" t="s">
+        <v>2741</v>
+      </c>
+      <c r="B1005" s="2" t="s">
+        <v>2638</v>
+      </c>
+      <c r="C1005" s="2" t="s">
+        <v>2673</v>
+      </c>
+      <c r="D1005" s="2" t="s">
+        <v>2674</v>
+      </c>
+      <c r="E1005" s="2" t="s">
+        <v>2670</v>
+      </c>
+      <c r="F1005" s="2" t="s">
+        <v>520</v>
+      </c>
+      <c r="G1005" s="2">
+        <v>69140</v>
+      </c>
+      <c r="H1005" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="I1005" s="2" t="s">
+        <v>2742</v>
+      </c>
+    </row>
+    <row r="1006" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A1006" s="2" t="s">
+        <v>2741</v>
+      </c>
+      <c r="B1006" s="2" t="s">
+        <v>2638</v>
+      </c>
+      <c r="C1006" s="2" t="s">
+        <v>2675</v>
+      </c>
+      <c r="D1006" s="2" t="s">
+        <v>2676</v>
+      </c>
+      <c r="E1006" s="2" t="s">
+        <v>2677</v>
+      </c>
+      <c r="F1006" s="2" t="s">
+        <v>520</v>
+      </c>
+      <c r="G1006" s="2">
+        <v>69033</v>
+      </c>
+      <c r="H1006" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="I1006" s="2" t="s">
+        <v>2742</v>
+      </c>
+    </row>
+    <row r="1007" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A1007" s="2" t="s">
+        <v>2741</v>
+      </c>
+      <c r="B1007" s="2" t="s">
+        <v>2638</v>
+      </c>
+      <c r="C1007" s="2" t="s">
+        <v>2678</v>
+      </c>
+      <c r="D1007" s="2" t="s">
+        <v>2679</v>
+      </c>
+      <c r="E1007" s="2" t="s">
+        <v>2677</v>
+      </c>
+      <c r="F1007" s="2" t="s">
+        <v>520</v>
+      </c>
+      <c r="G1007" s="2">
+        <v>69033</v>
+      </c>
+      <c r="H1007" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="I1007" s="2" t="s">
+        <v>2742</v>
+      </c>
+    </row>
+    <row r="1008" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A1008" s="2" t="s">
+        <v>2741</v>
+      </c>
+      <c r="B1008" s="2" t="s">
+        <v>2638</v>
+      </c>
+      <c r="C1008" s="2" t="s">
+        <v>2680</v>
+      </c>
+      <c r="D1008" s="2" t="s">
+        <v>2681</v>
+      </c>
+      <c r="E1008" s="2" t="s">
+        <v>2677</v>
+      </c>
+      <c r="F1008" s="2" t="s">
+        <v>520</v>
+      </c>
+      <c r="G1008" s="2">
+        <v>69033</v>
+      </c>
+      <c r="H1008" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="I1008" s="2" t="s">
+        <v>2742</v>
+      </c>
+    </row>
+    <row r="1009" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A1009" s="2" t="s">
+        <v>2741</v>
+      </c>
+      <c r="B1009" s="2" t="s">
+        <v>2638</v>
+      </c>
+      <c r="C1009" s="2" t="s">
+        <v>2682</v>
+      </c>
+      <c r="D1009" s="2" t="s">
+        <v>2683</v>
+      </c>
+      <c r="E1009" s="2" t="s">
+        <v>2677</v>
+      </c>
+      <c r="F1009" s="2" t="s">
+        <v>520</v>
+      </c>
+      <c r="G1009" s="2">
+        <v>69033</v>
+      </c>
+      <c r="H1009" s="2" t="s">
+        <v>2684</v>
+      </c>
+      <c r="I1009" s="2" t="s">
+        <v>2742</v>
+      </c>
+    </row>
+    <row r="1010" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A1010" s="2" t="s">
+        <v>2741</v>
+      </c>
+      <c r="B1010" s="2" t="s">
+        <v>2638</v>
+      </c>
+      <c r="C1010" s="2" t="s">
+        <v>2685</v>
+      </c>
+      <c r="D1010" s="2" t="s">
+        <v>2683</v>
+      </c>
+      <c r="E1010" s="2" t="s">
+        <v>2677</v>
+      </c>
+      <c r="F1010" s="2" t="s">
+        <v>520</v>
+      </c>
+      <c r="G1010" s="2">
+        <v>69033</v>
+      </c>
+      <c r="H1010" s="2" t="s">
+        <v>225</v>
+      </c>
+      <c r="I1010" s="2" t="s">
+        <v>2742</v>
+      </c>
+    </row>
+    <row r="1011" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A1011" s="2" t="s">
+        <v>2741</v>
+      </c>
+      <c r="B1011" s="2" t="s">
+        <v>2638</v>
+      </c>
+      <c r="C1011" s="2" t="s">
+        <v>2686</v>
+      </c>
+      <c r="D1011" s="2" t="s">
+        <v>2687</v>
+      </c>
+      <c r="E1011" s="2" t="s">
+        <v>2677</v>
+      </c>
+      <c r="F1011" s="2" t="s">
+        <v>520</v>
+      </c>
+      <c r="G1011" s="2">
+        <v>69033</v>
+      </c>
+      <c r="H1011" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="I1011" s="2" t="s">
+        <v>2742</v>
+      </c>
+    </row>
+    <row r="1012" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A1012" s="2" t="s">
+        <v>2741</v>
+      </c>
+      <c r="B1012" s="2" t="s">
+        <v>2638</v>
+      </c>
+      <c r="C1012" s="2" t="s">
+        <v>2688</v>
+      </c>
+      <c r="D1012" s="2" t="s">
+        <v>2689</v>
+      </c>
+      <c r="E1012" s="2" t="s">
+        <v>2677</v>
+      </c>
+      <c r="F1012" s="2" t="s">
+        <v>520</v>
+      </c>
+      <c r="G1012" s="2">
+        <v>69033</v>
+      </c>
+      <c r="H1012" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="I1012" s="2" t="s">
+        <v>2742</v>
+      </c>
+    </row>
+    <row r="1013" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A1013" s="2" t="s">
+        <v>2741</v>
+      </c>
+      <c r="B1013" s="2" t="s">
+        <v>2638</v>
+      </c>
+      <c r="C1013" s="2" t="s">
+        <v>2690</v>
+      </c>
+      <c r="D1013" s="2" t="s">
+        <v>2691</v>
+      </c>
+      <c r="E1013" s="2" t="s">
+        <v>249</v>
+      </c>
+      <c r="F1013" s="2" t="s">
+        <v>520</v>
+      </c>
+      <c r="G1013" s="2">
+        <v>69145</v>
+      </c>
+      <c r="H1013" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="I1013" s="2" t="s">
+        <v>2742</v>
+      </c>
+    </row>
+    <row r="1014" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A1014" s="2" t="s">
+        <v>2741</v>
+      </c>
+      <c r="B1014" s="2" t="s">
+        <v>2638</v>
+      </c>
+      <c r="C1014" s="2" t="s">
+        <v>2692</v>
+      </c>
+      <c r="D1014" s="2" t="s">
+        <v>2691</v>
+      </c>
+      <c r="E1014" s="2" t="s">
+        <v>249</v>
+      </c>
+      <c r="F1014" s="2" t="s">
+        <v>520</v>
+      </c>
+      <c r="G1014" s="2">
+        <v>69145</v>
+      </c>
+      <c r="H1014" s="2" t="s">
+        <v>1646</v>
+      </c>
+      <c r="I1014" s="2" t="s">
+        <v>2742</v>
+      </c>
+    </row>
+    <row r="1015" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A1015" s="2" t="s">
+        <v>2741</v>
+      </c>
+      <c r="B1015" s="2" t="s">
+        <v>2638</v>
+      </c>
+      <c r="C1015" s="2" t="s">
+        <v>2693</v>
+      </c>
+      <c r="D1015" s="2" t="s">
+        <v>2694</v>
+      </c>
+      <c r="E1015" s="2" t="s">
+        <v>249</v>
+      </c>
+      <c r="F1015" s="2" t="s">
+        <v>520</v>
+      </c>
+      <c r="G1015" s="2">
+        <v>69145</v>
+      </c>
+      <c r="H1015" s="2" t="s">
+        <v>2684</v>
+      </c>
+      <c r="I1015" s="2" t="s">
+        <v>2742</v>
+      </c>
+    </row>
+    <row r="1016" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A1016" s="2" t="s">
+        <v>2741</v>
+      </c>
+      <c r="B1016" s="2" t="s">
+        <v>2638</v>
+      </c>
+      <c r="C1016" s="2" t="s">
+        <v>2695</v>
+      </c>
+      <c r="D1016" s="2" t="s">
+        <v>2696</v>
+      </c>
+      <c r="E1016" s="2" t="s">
+        <v>2697</v>
+      </c>
+      <c r="F1016" s="2" t="s">
+        <v>520</v>
+      </c>
+      <c r="G1016" s="2">
+        <v>69149</v>
+      </c>
+      <c r="H1016" s="2" t="s">
+        <v>225</v>
+      </c>
+      <c r="I1016" s="2" t="s">
+        <v>2742</v>
+      </c>
+    </row>
+    <row r="1017" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A1017" s="2" t="s">
+        <v>2741</v>
+      </c>
+      <c r="B1017" s="2" t="s">
+        <v>2638</v>
+      </c>
+      <c r="C1017" s="2" t="s">
+        <v>2698</v>
+      </c>
+      <c r="D1017" s="2" t="s">
+        <v>2699</v>
+      </c>
+      <c r="E1017" s="2" t="s">
+        <v>2697</v>
+      </c>
+      <c r="F1017" s="2" t="s">
+        <v>520</v>
+      </c>
+      <c r="G1017" s="2">
+        <v>69149</v>
+      </c>
+      <c r="H1017" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="I1017" s="2" t="s">
+        <v>2742</v>
+      </c>
+    </row>
+    <row r="1018" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A1018" s="2" t="s">
+        <v>2741</v>
+      </c>
+      <c r="B1018" s="2" t="s">
+        <v>2638</v>
+      </c>
+      <c r="C1018" s="2" t="s">
+        <v>2700</v>
+      </c>
+      <c r="D1018" s="2" t="s">
+        <v>2701</v>
+      </c>
+      <c r="E1018" s="2" t="s">
+        <v>2702</v>
+      </c>
+      <c r="F1018" s="2" t="s">
+        <v>520</v>
+      </c>
+      <c r="G1018" s="2">
+        <v>69001</v>
+      </c>
+      <c r="H1018" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="I1018" s="2" t="s">
+        <v>2742</v>
+      </c>
+    </row>
+    <row r="1019" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A1019" s="2" t="s">
+        <v>2741</v>
+      </c>
+      <c r="B1019" s="2" t="s">
+        <v>2638</v>
+      </c>
+      <c r="C1019" s="2" t="s">
+        <v>2703</v>
+      </c>
+      <c r="D1019" s="2" t="s">
+        <v>2704</v>
+      </c>
+      <c r="E1019" s="2" t="s">
+        <v>2702</v>
+      </c>
+      <c r="F1019" s="2" t="s">
+        <v>520</v>
+      </c>
+      <c r="G1019" s="2">
+        <v>69001</v>
+      </c>
+      <c r="H1019" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="I1019" s="2" t="s">
+        <v>2742</v>
+      </c>
+    </row>
+    <row r="1020" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A1020" s="2" t="s">
+        <v>2741</v>
+      </c>
+      <c r="B1020" s="2" t="s">
+        <v>2638</v>
+      </c>
+      <c r="C1020" s="2" t="s">
+        <v>2705</v>
+      </c>
+      <c r="D1020" s="2" t="s">
+        <v>2706</v>
+      </c>
+      <c r="E1020" s="2" t="s">
+        <v>2702</v>
+      </c>
+      <c r="F1020" s="2" t="s">
+        <v>520</v>
+      </c>
+      <c r="G1020" s="2">
+        <v>69001</v>
+      </c>
+      <c r="H1020" s="2" t="s">
+        <v>1646</v>
+      </c>
+      <c r="I1020" s="2" t="s">
+        <v>2742</v>
+      </c>
+    </row>
+    <row r="1021" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A1021" s="2" t="s">
+        <v>2741</v>
+      </c>
+      <c r="B1021" s="2" t="s">
+        <v>2638</v>
+      </c>
+      <c r="C1021" s="2" t="s">
+        <v>2707</v>
+      </c>
+      <c r="D1021" s="2" t="s">
+        <v>2708</v>
+      </c>
+      <c r="E1021" s="2" t="s">
+        <v>2702</v>
+      </c>
+      <c r="F1021" s="2" t="s">
+        <v>520</v>
+      </c>
+      <c r="G1021" s="2">
+        <v>69001</v>
+      </c>
+      <c r="H1021" s="2" t="s">
+        <v>225</v>
+      </c>
+      <c r="I1021" s="2" t="s">
+        <v>2742</v>
+      </c>
+    </row>
+    <row r="1022" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A1022" s="2" t="s">
+        <v>2741</v>
+      </c>
+      <c r="B1022" s="2" t="s">
+        <v>2638</v>
+      </c>
+      <c r="C1022" s="2" t="s">
+        <v>2709</v>
+      </c>
+      <c r="D1022" s="2" t="s">
+        <v>2710</v>
+      </c>
+      <c r="E1022" s="2" t="s">
+        <v>2702</v>
+      </c>
+      <c r="F1022" s="2" t="s">
+        <v>520</v>
+      </c>
+      <c r="G1022" s="2">
+        <v>69001</v>
+      </c>
+      <c r="H1022" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="I1022" s="2" t="s">
+        <v>2742</v>
+      </c>
+    </row>
+    <row r="1023" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A1023" s="2" t="s">
+        <v>2741</v>
+      </c>
+      <c r="B1023" s="2" t="s">
+        <v>2638</v>
+      </c>
+      <c r="C1023" s="2" t="s">
+        <v>2711</v>
+      </c>
+      <c r="D1023" s="2" t="s">
+        <v>2712</v>
+      </c>
+      <c r="E1023" s="2" t="s">
+        <v>2713</v>
+      </c>
+      <c r="F1023" s="2" t="s">
+        <v>520</v>
+      </c>
+      <c r="G1023" s="2">
+        <v>69154</v>
+      </c>
+      <c r="H1023" s="2" t="s">
+        <v>225</v>
+      </c>
+      <c r="I1023" s="2" t="s">
+        <v>2742</v>
+      </c>
+    </row>
+    <row r="1024" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A1024" s="2" t="s">
+        <v>2741</v>
+      </c>
+      <c r="B1024" s="2" t="s">
+        <v>2638</v>
+      </c>
+      <c r="C1024" s="2" t="s">
+        <v>2714</v>
+      </c>
+      <c r="D1024" s="2" t="s">
+        <v>2715</v>
+      </c>
+      <c r="E1024" s="2" t="s">
+        <v>2716</v>
+      </c>
+      <c r="F1024" s="2" t="s">
+        <v>520</v>
+      </c>
+      <c r="G1024" s="2">
+        <v>69040</v>
+      </c>
+      <c r="H1024" s="2" t="s">
+        <v>225</v>
+      </c>
+      <c r="I1024" s="2" t="s">
+        <v>2742</v>
+      </c>
+    </row>
+    <row r="1025" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A1025" s="2" t="s">
+        <v>2741</v>
+      </c>
+      <c r="B1025" s="2" t="s">
+        <v>2638</v>
+      </c>
+      <c r="C1025" s="2" t="s">
+        <v>2717</v>
+      </c>
+      <c r="D1025" s="2" t="s">
+        <v>2718</v>
+      </c>
+      <c r="E1025" s="2" t="s">
+        <v>2719</v>
+      </c>
+      <c r="F1025" s="2" t="s">
+        <v>2647</v>
+      </c>
+      <c r="G1025" s="2">
+        <v>82082</v>
+      </c>
+      <c r="H1025" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="I1025" s="2" t="s">
+        <v>2742</v>
+      </c>
+    </row>
+    <row r="1026" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A1026" s="2" t="s">
+        <v>2741</v>
+      </c>
+      <c r="B1026" s="2" t="s">
+        <v>2638</v>
+      </c>
+      <c r="C1026" s="2" t="s">
+        <v>2720</v>
+      </c>
+      <c r="D1026" s="2" t="s">
+        <v>2721</v>
+      </c>
+      <c r="E1026" s="2" t="s">
+        <v>2719</v>
+      </c>
+      <c r="F1026" s="2" t="s">
+        <v>2647</v>
+      </c>
+      <c r="G1026" s="2">
+        <v>82082</v>
+      </c>
+      <c r="H1026" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="I1026" s="2" t="s">
+        <v>2742</v>
+      </c>
+    </row>
+    <row r="1027" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A1027" s="2" t="s">
+        <v>2741</v>
+      </c>
+      <c r="B1027" s="2" t="s">
+        <v>2638</v>
+      </c>
+      <c r="C1027" s="2" t="s">
+        <v>2722</v>
+      </c>
+      <c r="D1027" s="2" t="s">
+        <v>2723</v>
+      </c>
+      <c r="E1027" s="2" t="s">
+        <v>2719</v>
+      </c>
+      <c r="F1027" s="2" t="s">
+        <v>2647</v>
+      </c>
+      <c r="G1027" s="2">
+        <v>82082</v>
+      </c>
+      <c r="H1027" s="2" t="s">
+        <v>225</v>
+      </c>
+      <c r="I1027" s="2" t="s">
+        <v>2742</v>
+      </c>
+    </row>
+    <row r="1028" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A1028" s="2" t="s">
+        <v>2741</v>
+      </c>
+      <c r="B1028" s="2" t="s">
+        <v>2638</v>
+      </c>
+      <c r="C1028" s="2" t="s">
+        <v>2724</v>
+      </c>
+      <c r="D1028" s="2" t="s">
+        <v>2725</v>
+      </c>
+      <c r="E1028" s="2" t="s">
+        <v>2726</v>
+      </c>
+      <c r="F1028" s="2" t="s">
+        <v>520</v>
+      </c>
+      <c r="G1028" s="2">
+        <v>69156</v>
+      </c>
+      <c r="H1028" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="I1028" s="2" t="s">
+        <v>2742</v>
+      </c>
+    </row>
+    <row r="1029" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A1029" s="2" t="s">
+        <v>2741</v>
+      </c>
+      <c r="B1029" s="2" t="s">
+        <v>2638</v>
+      </c>
+      <c r="C1029" s="2" t="s">
+        <v>2727</v>
+      </c>
+      <c r="D1029" s="2" t="s">
+        <v>2728</v>
+      </c>
+      <c r="E1029" s="2" t="s">
+        <v>2729</v>
+      </c>
+      <c r="F1029" s="2" t="s">
+        <v>520</v>
+      </c>
+      <c r="G1029" s="2">
+        <v>69162</v>
+      </c>
+      <c r="H1029" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="I1029" s="2" t="s">
+        <v>2742</v>
+      </c>
+    </row>
+    <row r="1030" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A1030" s="2" t="s">
+        <v>2741</v>
+      </c>
+      <c r="B1030" s="2" t="s">
+        <v>2638</v>
+      </c>
+      <c r="C1030" s="2" t="s">
+        <v>2730</v>
+      </c>
+      <c r="D1030" s="2" t="s">
+        <v>2731</v>
+      </c>
+      <c r="E1030" s="2" t="s">
+        <v>2729</v>
+      </c>
+      <c r="F1030" s="2" t="s">
+        <v>520</v>
+      </c>
+      <c r="G1030" s="2">
+        <v>69162</v>
+      </c>
+      <c r="H1030" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="I1030" s="2" t="s">
+        <v>2742</v>
+      </c>
+    </row>
+    <row r="1031" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A1031" s="2" t="s">
+        <v>2741</v>
+      </c>
+      <c r="B1031" s="2" t="s">
+        <v>2638</v>
+      </c>
+      <c r="C1031" s="2" t="s">
+        <v>2732</v>
+      </c>
+      <c r="D1031" s="2" t="s">
+        <v>2733</v>
+      </c>
+      <c r="E1031" s="2" t="s">
+        <v>2734</v>
+      </c>
+      <c r="F1031" s="2" t="s">
+        <v>520</v>
+      </c>
+      <c r="G1031" s="2">
+        <v>69168</v>
+      </c>
+      <c r="H1031" s="2" t="s">
+        <v>225</v>
+      </c>
+      <c r="I1031" s="2" t="s">
+        <v>2742</v>
+      </c>
+    </row>
+    <row r="1032" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A1032" s="2" t="s">
+        <v>2741</v>
+      </c>
+      <c r="B1032" s="2" t="s">
+        <v>2638</v>
+      </c>
+      <c r="C1032" s="2" t="s">
+        <v>2735</v>
+      </c>
+      <c r="D1032" s="2" t="s">
+        <v>2736</v>
+      </c>
+      <c r="E1032" s="2" t="s">
+        <v>2737</v>
+      </c>
+      <c r="F1032" s="2" t="s">
+        <v>520</v>
+      </c>
+      <c r="G1032" s="2">
+        <v>69045</v>
+      </c>
+      <c r="H1032" s="2" t="s">
+        <v>225</v>
+      </c>
+      <c r="I1032" s="2" t="s">
+        <v>2742</v>
+      </c>
+    </row>
+    <row r="1033" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A1033" s="2" t="s">
+        <v>2741</v>
+      </c>
+      <c r="B1033" s="2" t="s">
+        <v>2638</v>
+      </c>
+      <c r="C1033" s="2" t="s">
+        <v>2738</v>
+      </c>
+      <c r="D1033" s="2" t="s">
+        <v>2739</v>
+      </c>
+      <c r="E1033" s="2" t="s">
+        <v>2740</v>
+      </c>
+      <c r="F1033" s="2" t="s">
+        <v>2647</v>
+      </c>
+      <c r="G1033" s="2">
+        <v>82201</v>
+      </c>
+      <c r="H1033" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="I1033" s="2" t="s">
+        <v>2742</v>
       </c>
     </row>
   </sheetData>
@@ -37216,6 +38752,15 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <lcf76f155ced4ddcb4097134ff3c332f xmlns="7cecf09e-87d6-4345-a370-97524ef8da64">
@@ -37223,15 +38768,6 @@
     </lcf76f155ced4ddcb4097134ff3c332f>
   </documentManagement>
 </p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -37253,6 +38789,14 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{10CF58AA-00EF-4BDF-A97C-BB1A0168CFB8}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9BF1610B-6E8D-417B-A267-064FFADDBB14}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
@@ -37260,12 +38804,4 @@
     <ds:schemaRef ds:uri="7cecf09e-87d6-4345-a370-97524ef8da64"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{10CF58AA-00EF-4BDF-A97C-BB1A0168CFB8}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
✅ Fix kingpin ContactName + true-coords stops
</commit_message>
<xml_diff>
--- a/data/retailers.xlsx
+++ b/data/retailers.xlsx
@@ -909,7 +909,7 @@
       </c>
       <c r="H11" t="inlineStr">
         <is>
-          <t>Corporate HQ</t>
+          <t>Regional HQ</t>
         </is>
       </c>
       <c r="I11" t="inlineStr">
@@ -1629,7 +1629,7 @@
       </c>
       <c r="H27" t="inlineStr">
         <is>
-          <t>Corporate HQ</t>
+          <t>Regional HQ</t>
         </is>
       </c>
       <c r="I27" t="inlineStr">
@@ -1966,7 +1966,7 @@
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>Cherokee – Corporate HQ</t>
+          <t>Cherokee – Regional HQ</t>
         </is>
       </c>
       <c r="D35" t="inlineStr">
@@ -1989,7 +1989,7 @@
       </c>
       <c r="H35" t="inlineStr">
         <is>
-          <t>Corporate HQ</t>
+          <t>Regional HQ</t>
         </is>
       </c>
       <c r="I35" t="inlineStr">
@@ -2934,7 +2934,7 @@
       </c>
       <c r="H56" t="inlineStr">
         <is>
-          <t>Corporate HQ</t>
+          <t>Regional HQ</t>
         </is>
       </c>
       <c r="I56" t="inlineStr">
@@ -5589,7 +5589,7 @@
       </c>
       <c r="H115" t="inlineStr">
         <is>
-          <t>Corporate HQ</t>
+          <t>Regional HQ</t>
         </is>
       </c>
       <c r="I115" t="inlineStr">
@@ -7119,7 +7119,7 @@
       </c>
       <c r="H149" t="inlineStr">
         <is>
-          <t>Corporate HQ</t>
+          <t>Regional HQ</t>
         </is>
       </c>
       <c r="I149" t="inlineStr">
@@ -7884,7 +7884,7 @@
       </c>
       <c r="H166" t="inlineStr">
         <is>
-          <t>Corporate HQ</t>
+          <t>Regional HQ</t>
         </is>
       </c>
       <c r="I166" t="inlineStr">
@@ -7974,7 +7974,7 @@
       </c>
       <c r="H168" t="inlineStr">
         <is>
-          <t>Corporate HQ</t>
+          <t>Regional HQ</t>
         </is>
       </c>
       <c r="I168" t="inlineStr">
@@ -8469,7 +8469,7 @@
       </c>
       <c r="H179" t="inlineStr">
         <is>
-          <t>Corporate HQ</t>
+          <t>Regional HQ</t>
         </is>
       </c>
       <c r="I179" t="inlineStr">
@@ -11844,7 +11844,7 @@
       </c>
       <c r="H254" t="inlineStr">
         <is>
-          <t>Corporate HQ</t>
+          <t>Regional HQ</t>
         </is>
       </c>
       <c r="I254" t="inlineStr">
@@ -11979,7 +11979,7 @@
       </c>
       <c r="H257" t="inlineStr">
         <is>
-          <t>Corporate HQ</t>
+          <t>Regional HQ</t>
         </is>
       </c>
       <c r="I257" t="inlineStr">
@@ -12969,7 +12969,7 @@
       </c>
       <c r="H279" t="inlineStr">
         <is>
-          <t>Corporate HQ, Grain</t>
+          <t>Regional HQ, Grain</t>
         </is>
       </c>
       <c r="I279" t="inlineStr">
@@ -13059,7 +13059,7 @@
       </c>
       <c r="H281" t="inlineStr">
         <is>
-          <t>Corporate HQ</t>
+          <t>Regional HQ</t>
         </is>
       </c>
       <c r="I281" t="inlineStr">
@@ -13194,7 +13194,7 @@
       </c>
       <c r="H284" t="inlineStr">
         <is>
-          <t>Corporate HQ</t>
+          <t>Regional HQ</t>
         </is>
       </c>
       <c r="I284" t="inlineStr">
@@ -13464,7 +13464,7 @@
       </c>
       <c r="H290" t="inlineStr">
         <is>
-          <t>Corporate HQ</t>
+          <t>Regional HQ</t>
         </is>
       </c>
       <c r="I290" t="inlineStr">
@@ -15309,7 +15309,7 @@
       </c>
       <c r="H331" t="inlineStr">
         <is>
-          <t>Corporate HQ</t>
+          <t>Regional HQ</t>
         </is>
       </c>
       <c r="I331" t="inlineStr">
@@ -16074,7 +16074,7 @@
       </c>
       <c r="H348" t="inlineStr">
         <is>
-          <t>Corporate HQ</t>
+          <t>Regional HQ</t>
         </is>
       </c>
       <c r="I348" t="inlineStr">
@@ -17019,7 +17019,7 @@
       </c>
       <c r="H369" t="inlineStr">
         <is>
-          <t>Corporate HQ, Grain</t>
+          <t>Regional HQ, Grain</t>
         </is>
       </c>
       <c r="I369" t="inlineStr">
@@ -17469,7 +17469,7 @@
       </c>
       <c r="H379" t="inlineStr">
         <is>
-          <t>Corporate HQ</t>
+          <t>Regional HQ</t>
         </is>
       </c>
       <c r="I379" t="inlineStr">
@@ -18099,7 +18099,7 @@
       </c>
       <c r="H393" t="inlineStr">
         <is>
-          <t>Corporate HQ</t>
+          <t>Regional HQ</t>
         </is>
       </c>
       <c r="I393" t="inlineStr">
@@ -19269,7 +19269,7 @@
       </c>
       <c r="H419" t="inlineStr">
         <is>
-          <t>Corporate HQ</t>
+          <t>Regional HQ</t>
         </is>
       </c>
       <c r="I419" t="inlineStr">
@@ -19764,7 +19764,7 @@
       </c>
       <c r="H430" t="inlineStr">
         <is>
-          <t>Corporate HQ</t>
+          <t>Regional HQ</t>
         </is>
       </c>
       <c r="I430" t="inlineStr">
@@ -20619,7 +20619,7 @@
       </c>
       <c r="H449" t="inlineStr">
         <is>
-          <t>Corporate HQ</t>
+          <t>Regional HQ</t>
         </is>
       </c>
       <c r="I449" t="inlineStr">
@@ -20934,7 +20934,7 @@
       </c>
       <c r="H456" t="inlineStr">
         <is>
-          <t>Corporate HQ</t>
+          <t>Regional HQ</t>
         </is>
       </c>
       <c r="I456" t="inlineStr">
@@ -21159,7 +21159,7 @@
       </c>
       <c r="H461" t="inlineStr">
         <is>
-          <t>Corporate HQ</t>
+          <t>Regional HQ</t>
         </is>
       </c>
       <c r="I461" t="inlineStr">
@@ -21744,7 +21744,7 @@
       </c>
       <c r="H474" t="inlineStr">
         <is>
-          <t>Corporate HQ</t>
+          <t>Regional HQ</t>
         </is>
       </c>
       <c r="I474" t="inlineStr">
@@ -22914,7 +22914,7 @@
       </c>
       <c r="H500" t="inlineStr">
         <is>
-          <t>Corporate HQ</t>
+          <t>Regional HQ</t>
         </is>
       </c>
       <c r="I500" t="inlineStr">
@@ -23049,7 +23049,7 @@
       </c>
       <c r="H503" t="inlineStr">
         <is>
-          <t>Corporate HQ</t>
+          <t>Regional HQ</t>
         </is>
       </c>
       <c r="I503" t="inlineStr">
@@ -24084,7 +24084,7 @@
       </c>
       <c r="H526" t="inlineStr">
         <is>
-          <t>Corporate HQ</t>
+          <t>Regional HQ</t>
         </is>
       </c>
       <c r="I526" t="inlineStr">
@@ -24174,7 +24174,7 @@
       </c>
       <c r="H528" t="inlineStr">
         <is>
-          <t>Corporate HQ</t>
+          <t>Regional HQ</t>
         </is>
       </c>
       <c r="I528" t="inlineStr">
@@ -25254,7 +25254,7 @@
       </c>
       <c r="H552" t="inlineStr">
         <is>
-          <t>Corporate HQ, C-Store/Service/Energy</t>
+          <t>Regional HQ, C-Store/Service/Energy</t>
         </is>
       </c>
       <c r="I552" t="inlineStr">
@@ -25614,7 +25614,7 @@
       </c>
       <c r="H560" t="inlineStr">
         <is>
-          <t>Corporate HQ</t>
+          <t>Regional HQ</t>
         </is>
       </c>
       <c r="I560" t="inlineStr">
@@ -26424,7 +26424,7 @@
       </c>
       <c r="H578" t="inlineStr">
         <is>
-          <t>Corporate HQ</t>
+          <t>Regional HQ</t>
         </is>
       </c>
       <c r="I578" t="inlineStr">
@@ -26919,7 +26919,7 @@
       </c>
       <c r="H589" t="inlineStr">
         <is>
-          <t>Corporate HQ</t>
+          <t>Regional HQ</t>
         </is>
       </c>
       <c r="I589" t="inlineStr">
@@ -27819,7 +27819,7 @@
       </c>
       <c r="H609" t="inlineStr">
         <is>
-          <t>Corporate HQ</t>
+          <t>Regional HQ</t>
         </is>
       </c>
       <c r="I609" t="inlineStr">
@@ -27864,7 +27864,7 @@
       </c>
       <c r="H610" t="inlineStr">
         <is>
-          <t>Corporate HQ</t>
+          <t>Regional HQ</t>
         </is>
       </c>
       <c r="I610" t="inlineStr">
@@ -27999,7 +27999,7 @@
       </c>
       <c r="H613" t="inlineStr">
         <is>
-          <t>Corporate HQ</t>
+          <t>Regional HQ</t>
         </is>
       </c>
       <c r="I613" t="inlineStr">
@@ -29034,7 +29034,7 @@
       </c>
       <c r="H636" t="inlineStr">
         <is>
-          <t>Corporate HQ</t>
+          <t>Regional HQ</t>
         </is>
       </c>
       <c r="I636" t="inlineStr">
@@ -30159,7 +30159,7 @@
       </c>
       <c r="H661" t="inlineStr">
         <is>
-          <t>Corporate HQ</t>
+          <t>Regional HQ</t>
         </is>
       </c>
       <c r="I661" t="inlineStr">
@@ -30676,7 +30676,7 @@
       </c>
       <c r="C673" t="inlineStr">
         <is>
-          <t>Dunlap Corporate HQ</t>
+          <t>Dunlap Regional HQ</t>
         </is>
       </c>
       <c r="D673" t="inlineStr">
@@ -30699,7 +30699,7 @@
       </c>
       <c r="H673" t="inlineStr">
         <is>
-          <t>Corporate HQ</t>
+          <t>Regional HQ</t>
         </is>
       </c>
       <c r="I673" t="inlineStr">
@@ -31374,7 +31374,7 @@
       </c>
       <c r="H688" t="inlineStr">
         <is>
-          <t>Corporate HQ</t>
+          <t>Regional HQ</t>
         </is>
       </c>
       <c r="I688" t="inlineStr">
@@ -31599,7 +31599,7 @@
       </c>
       <c r="H693" t="inlineStr">
         <is>
-          <t>Corporate HQ</t>
+          <t>Regional HQ</t>
         </is>
       </c>
       <c r="I693" t="inlineStr">
@@ -32184,7 +32184,7 @@
       </c>
       <c r="H706" t="inlineStr">
         <is>
-          <t>Corporate HQ</t>
+          <t>Regional HQ</t>
         </is>
       </c>
       <c r="I706" t="inlineStr">
@@ -33421,7 +33421,7 @@
       </c>
       <c r="C734" t="inlineStr">
         <is>
-          <t>Imperial – Corporate HQ / Main Office</t>
+          <t>Imperial – Regional HQ / Main Office</t>
         </is>
       </c>
       <c r="D734" t="inlineStr">
@@ -33444,7 +33444,7 @@
       </c>
       <c r="H734" t="inlineStr">
         <is>
-          <t>Corporate HQ</t>
+          <t>Regional HQ</t>
         </is>
       </c>
       <c r="I734" t="inlineStr">
@@ -36279,7 +36279,7 @@
       </c>
       <c r="H797" t="inlineStr">
         <is>
-          <t>Corporate HQ</t>
+          <t>Regional HQ</t>
         </is>
       </c>
       <c r="I797" t="inlineStr">
@@ -37989,7 +37989,7 @@
       </c>
       <c r="H835" t="inlineStr">
         <is>
-          <t>Corporate HQ</t>
+          <t>Regional HQ</t>
         </is>
       </c>
       <c r="I835" t="inlineStr">
@@ -38259,7 +38259,7 @@
       </c>
       <c r="H841" t="inlineStr">
         <is>
-          <t>Corporate HQ</t>
+          <t>Regional HQ</t>
         </is>
       </c>
       <c r="I841" t="inlineStr">
@@ -38349,7 +38349,7 @@
       </c>
       <c r="H843" t="inlineStr">
         <is>
-          <t>Corporate HQ</t>
+          <t>Regional HQ</t>
         </is>
       </c>
       <c r="I843" t="inlineStr">
@@ -39384,7 +39384,7 @@
       </c>
       <c r="H866" t="inlineStr">
         <is>
-          <t>Corporate HQ</t>
+          <t>Regional HQ</t>
         </is>
       </c>
       <c r="I866" t="inlineStr">
@@ -39654,7 +39654,7 @@
       </c>
       <c r="H872" t="inlineStr">
         <is>
-          <t>Corporate HQ</t>
+          <t>Regional HQ</t>
         </is>
       </c>
       <c r="I872" t="inlineStr">
@@ -43569,7 +43569,7 @@
       </c>
       <c r="H959" t="inlineStr">
         <is>
-          <t>Corporate HQ</t>
+          <t>Regional HQ</t>
         </is>
       </c>
       <c r="I959" t="inlineStr">
@@ -44559,7 +44559,7 @@
       </c>
       <c r="H981" t="inlineStr">
         <is>
-          <t>Corporate HQ</t>
+          <t>Regional HQ</t>
         </is>
       </c>
       <c r="I981" t="inlineStr">
@@ -45009,7 +45009,7 @@
       </c>
       <c r="H991" t="inlineStr">
         <is>
-          <t>Corporate HQ</t>
+          <t>Regional HQ</t>
         </is>
       </c>
       <c r="I991" t="inlineStr">
@@ -45504,7 +45504,7 @@
       </c>
       <c r="H1002" t="inlineStr">
         <is>
-          <t>Corporate HQ</t>
+          <t>Regional HQ</t>
         </is>
       </c>
       <c r="I1002" t="inlineStr">
@@ -45684,7 +45684,7 @@
       </c>
       <c r="H1006" t="inlineStr">
         <is>
-          <t>Corporate HQ</t>
+          <t>Regional HQ</t>
         </is>
       </c>
       <c r="I1006" t="inlineStr">
@@ -45819,7 +45819,7 @@
       </c>
       <c r="H1009" t="inlineStr">
         <is>
-          <t>Corporate HQ</t>
+          <t>Regional HQ</t>
         </is>
       </c>
       <c r="I1009" t="inlineStr">
@@ -46044,7 +46044,7 @@
       </c>
       <c r="H1014" t="inlineStr">
         <is>
-          <t>Corporate HQ</t>
+          <t>Regional HQ</t>
         </is>
       </c>
       <c r="I1014" t="inlineStr">
@@ -46494,7 +46494,7 @@
       </c>
       <c r="H1024" t="inlineStr">
         <is>
-          <t>Corporate HQ</t>
+          <t>Regional HQ</t>
         </is>
       </c>
       <c r="I1024" t="inlineStr">
@@ -47326,7 +47326,7 @@
       </c>
       <c r="C1043" t="inlineStr">
         <is>
-          <t>Elsie Corporate HQ</t>
+          <t>Elsie Regional HQ</t>
         </is>
       </c>
       <c r="D1043" t="inlineStr">
@@ -47349,7 +47349,7 @@
       </c>
       <c r="H1043" t="inlineStr">
         <is>
-          <t>Corporate HQ</t>
+          <t>Regional HQ</t>
         </is>
       </c>
       <c r="I1043" t="inlineStr">
@@ -47394,7 +47394,7 @@
       </c>
       <c r="H1044" t="inlineStr">
         <is>
-          <t>Corporate HQ</t>
+          <t>Regional HQ</t>
         </is>
       </c>
       <c r="I1044" t="inlineStr"/>
@@ -47435,7 +47435,7 @@
       </c>
       <c r="H1045" t="inlineStr">
         <is>
-          <t>Corporate HQ</t>
+          <t>Regional HQ</t>
         </is>
       </c>
       <c r="I1045" t="inlineStr">
@@ -47975,7 +47975,7 @@
       </c>
       <c r="H1057" t="inlineStr">
         <is>
-          <t>Corporate HQ</t>
+          <t>Regional HQ</t>
         </is>
       </c>
       <c r="I1057" t="inlineStr">
@@ -48335,7 +48335,7 @@
       </c>
       <c r="H1065" t="inlineStr">
         <is>
-          <t>Corporate HQ</t>
+          <t>Regional HQ</t>
         </is>
       </c>
       <c r="I1065" t="inlineStr">
@@ -48695,7 +48695,7 @@
       </c>
       <c r="H1073" t="inlineStr">
         <is>
-          <t>Corporate HQ</t>
+          <t>Regional HQ</t>
         </is>
       </c>
       <c r="I1073" t="inlineStr">
@@ -51539,7 +51539,7 @@
       </c>
       <c r="H1141" t="inlineStr">
         <is>
-          <t>Corporate HQ</t>
+          <t>Regional HQ</t>
         </is>
       </c>
       <c r="I1141" t="inlineStr">
@@ -51809,7 +51809,7 @@
       </c>
       <c r="H1147" t="inlineStr">
         <is>
-          <t>Corporate HQ</t>
+          <t>Regional HQ</t>
         </is>
       </c>
       <c r="I1147" t="inlineStr"/>
@@ -51895,7 +51895,7 @@
       </c>
       <c r="H1149" t="inlineStr">
         <is>
-          <t>Corporate HQ</t>
+          <t>Regional HQ</t>
         </is>
       </c>
       <c r="I1149" t="inlineStr">
@@ -52165,7 +52165,7 @@
       </c>
       <c r="H1155" t="inlineStr">
         <is>
-          <t>Corporate HQ</t>
+          <t>Regional HQ</t>
         </is>
       </c>
       <c r="I1155" t="inlineStr">
@@ -53515,7 +53515,7 @@
       </c>
       <c r="H1185" t="inlineStr">
         <is>
-          <t>Corporate HQ</t>
+          <t>Regional HQ</t>
         </is>
       </c>
       <c r="I1185" t="inlineStr">
@@ -54280,7 +54280,7 @@
       </c>
       <c r="H1202" t="inlineStr">
         <is>
-          <t>Corporate HQ</t>
+          <t>Regional HQ</t>
         </is>
       </c>
       <c r="I1202" t="inlineStr">
@@ -54325,7 +54325,7 @@
       </c>
       <c r="H1203" t="inlineStr">
         <is>
-          <t>Corporate HQ</t>
+          <t>Regional HQ</t>
         </is>
       </c>
       <c r="I1203" t="inlineStr">
@@ -55855,7 +55855,7 @@
       </c>
       <c r="H1237" t="inlineStr">
         <is>
-          <t>Corporate HQ</t>
+          <t>Regional HQ</t>
         </is>
       </c>
       <c r="I1237" t="inlineStr">
@@ -56440,7 +56440,7 @@
       </c>
       <c r="H1250" t="inlineStr">
         <is>
-          <t>Corporate HQ</t>
+          <t>Regional HQ</t>
         </is>
       </c>
       <c r="I1250" t="inlineStr">
@@ -57385,7 +57385,7 @@
       </c>
       <c r="H1271" t="inlineStr">
         <is>
-          <t>Corporate HQ</t>
+          <t>Regional HQ</t>
         </is>
       </c>
       <c r="I1271" t="inlineStr">
@@ -58870,7 +58870,7 @@
       </c>
       <c r="H1304" t="inlineStr">
         <is>
-          <t>Corporate HQ</t>
+          <t>Regional HQ</t>
         </is>
       </c>
       <c r="I1304" t="inlineStr">
@@ -59500,7 +59500,7 @@
       </c>
       <c r="H1318" t="inlineStr">
         <is>
-          <t>Corporate HQ</t>
+          <t>Regional HQ</t>
         </is>
       </c>
       <c r="I1318" t="inlineStr">
@@ -59545,7 +59545,7 @@
       </c>
       <c r="H1319" t="inlineStr">
         <is>
-          <t>Corporate HQ</t>
+          <t>Regional HQ</t>
         </is>
       </c>
       <c r="I1319" t="inlineStr">
@@ -61930,7 +61930,7 @@
       </c>
       <c r="H1372" t="inlineStr">
         <is>
-          <t>Corporate HQ</t>
+          <t>Regional HQ</t>
         </is>
       </c>
       <c r="I1372" t="inlineStr">
@@ -62020,7 +62020,7 @@
       </c>
       <c r="H1374" t="inlineStr">
         <is>
-          <t>Corporate HQ</t>
+          <t>Regional HQ</t>
         </is>
       </c>
       <c r="I1374" t="inlineStr">
@@ -62470,7 +62470,7 @@
       </c>
       <c r="H1384" t="inlineStr">
         <is>
-          <t>Corporate HQ</t>
+          <t>Regional HQ</t>
         </is>
       </c>
       <c r="I1384" t="inlineStr">
@@ -62785,7 +62785,7 @@
       </c>
       <c r="H1391" t="inlineStr">
         <is>
-          <t>Corporate HQ</t>
+          <t>Regional HQ</t>
         </is>
       </c>
       <c r="I1391" t="inlineStr">
@@ -63595,7 +63595,7 @@
       </c>
       <c r="H1409" t="inlineStr">
         <is>
-          <t>Corporate HQ</t>
+          <t>Regional HQ</t>
         </is>
       </c>
       <c r="I1409" t="inlineStr">
@@ -63730,7 +63730,7 @@
       </c>
       <c r="H1412" t="inlineStr">
         <is>
-          <t>Corporate HQ</t>
+          <t>Regional HQ</t>
         </is>
       </c>
       <c r="I1412" t="inlineStr">
@@ -63775,7 +63775,7 @@
       </c>
       <c r="H1413" t="inlineStr">
         <is>
-          <t>Corporate HQ</t>
+          <t>Regional HQ</t>
         </is>
       </c>
       <c r="I1413" t="inlineStr">
@@ -64135,7 +64135,7 @@
       </c>
       <c r="H1421" t="inlineStr">
         <is>
-          <t>Corporate HQ</t>
+          <t>Regional HQ</t>
         </is>
       </c>
       <c r="I1421" t="inlineStr">
@@ -64180,7 +64180,7 @@
       </c>
       <c r="H1422" t="inlineStr">
         <is>
-          <t>Corporate HQ</t>
+          <t>Regional HQ</t>
         </is>
       </c>
       <c r="I1422" t="inlineStr">
@@ -64900,7 +64900,7 @@
       </c>
       <c r="H1438" t="inlineStr">
         <is>
-          <t>Corporate HQ</t>
+          <t>Regional HQ</t>
         </is>
       </c>
       <c r="I1438" t="inlineStr">
@@ -64945,7 +64945,7 @@
       </c>
       <c r="H1439" t="inlineStr">
         <is>
-          <t>Corporate HQ</t>
+          <t>Regional HQ</t>
         </is>
       </c>
       <c r="I1439" t="inlineStr">
@@ -65665,7 +65665,7 @@
       </c>
       <c r="H1455" t="inlineStr">
         <is>
-          <t>Corporate HQ</t>
+          <t>Regional HQ</t>
         </is>
       </c>
       <c r="I1455" t="inlineStr">
@@ -66275,7 +66275,7 @@
       </c>
       <c r="H1469" t="inlineStr">
         <is>
-          <t>Corporate HQ</t>
+          <t>Regional HQ</t>
         </is>
       </c>
       <c r="I1469" t="inlineStr">
@@ -66824,7 +66824,7 @@
       </c>
       <c r="H1482" t="inlineStr">
         <is>
-          <t>Corporate HQ</t>
+          <t>Regional HQ</t>
         </is>
       </c>
       <c r="I1482" t="inlineStr">
@@ -67094,7 +67094,7 @@
       </c>
       <c r="H1488" t="inlineStr">
         <is>
-          <t>Corporate HQ</t>
+          <t>Regional HQ</t>
         </is>
       </c>
       <c r="I1488" t="inlineStr">
@@ -67904,7 +67904,7 @@
       </c>
       <c r="H1506" t="inlineStr">
         <is>
-          <t>Corporate HQ</t>
+          <t>Regional HQ</t>
         </is>
       </c>
       <c r="I1506" t="inlineStr">
@@ -68219,7 +68219,7 @@
       </c>
       <c r="H1513" t="inlineStr">
         <is>
-          <t>Corporate HQ</t>
+          <t>Regional HQ</t>
         </is>
       </c>
       <c r="I1513" t="inlineStr">
@@ -69119,7 +69119,7 @@
       </c>
       <c r="H1533" t="inlineStr">
         <is>
-          <t>Corporate HQ</t>
+          <t>Regional HQ</t>
         </is>
       </c>
       <c r="I1533" t="inlineStr">
@@ -69614,7 +69614,7 @@
       </c>
       <c r="H1544" t="inlineStr">
         <is>
-          <t>Corporate HQ</t>
+          <t>Regional HQ</t>
         </is>
       </c>
       <c r="I1544" t="inlineStr">
@@ -69839,7 +69839,7 @@
       </c>
       <c r="H1549" t="inlineStr">
         <is>
-          <t>Corporate HQ</t>
+          <t>Regional HQ</t>
         </is>
       </c>
       <c r="I1549" t="inlineStr">
@@ -70334,7 +70334,7 @@
       </c>
       <c r="H1560" t="inlineStr">
         <is>
-          <t>Corporate HQ</t>
+          <t>Regional HQ</t>
         </is>
       </c>
       <c r="I1560" t="inlineStr">
@@ -70739,7 +70739,7 @@
       </c>
       <c r="H1569" t="inlineStr">
         <is>
-          <t>Corporate HQ</t>
+          <t>Regional HQ</t>
         </is>
       </c>
       <c r="I1569" t="inlineStr">

</xml_diff>

<commit_message>
✅ Retailers pipeline fixed (Landus Category) + rebuild geojson
</commit_message>
<xml_diff>
--- a/data/retailers.xlsx
+++ b/data/retailers.xlsx
@@ -1,13 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -436,7 +436,7 @@
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>Long Name</t>
+          <t>LongName</t>
         </is>
       </c>
       <c r="B1" s="1" t="inlineStr">
@@ -32229,7 +32229,7 @@
       </c>
       <c r="H707" t="inlineStr">
         <is>
-          <t xml:space="preserve">Agronomy, </t>
+          <t>Agronomy,</t>
         </is>
       </c>
       <c r="I707" t="inlineStr">
@@ -49143,7 +49143,11 @@
       <c r="G1083" t="n">
         <v>50002</v>
       </c>
-      <c r="H1083" t="inlineStr"/>
+      <c r="H1083" t="inlineStr">
+        <is>
+          <t>Grain/Feed</t>
+        </is>
+      </c>
       <c r="I1083" t="inlineStr">
         <is>
           <t>IAP</t>
@@ -49184,7 +49188,11 @@
       <c r="G1084" t="n">
         <v>50022</v>
       </c>
-      <c r="H1084" t="inlineStr"/>
+      <c r="H1084" t="inlineStr">
+        <is>
+          <t>Agronomy, Grain/Feed</t>
+        </is>
+      </c>
       <c r="I1084" t="inlineStr">
         <is>
           <t>IAP</t>
@@ -49225,7 +49233,11 @@
       <c r="G1085" t="n">
         <v>50029</v>
       </c>
-      <c r="H1085" t="inlineStr"/>
+      <c r="H1085" t="inlineStr">
+        <is>
+          <t>Agronomy, Grain/Feed</t>
+        </is>
+      </c>
       <c r="I1085" t="inlineStr">
         <is>
           <t>IAP</t>
@@ -49266,7 +49278,11 @@
       <c r="G1086" t="n">
         <v>50031</v>
       </c>
-      <c r="H1086" t="inlineStr"/>
+      <c r="H1086" t="inlineStr">
+        <is>
+          <t>Grain/Feed</t>
+        </is>
+      </c>
       <c r="I1086" t="inlineStr">
         <is>
           <t>IAP</t>
@@ -49307,7 +49323,11 @@
       <c r="G1087" t="n">
         <v>50036</v>
       </c>
-      <c r="H1087" t="inlineStr"/>
+      <c r="H1087" t="inlineStr">
+        <is>
+          <t>Agronomy</t>
+        </is>
+      </c>
       <c r="I1087" t="inlineStr">
         <is>
           <t>IAP</t>
@@ -49348,7 +49368,11 @@
       <c r="G1088" t="n">
         <v>50036</v>
       </c>
-      <c r="H1088" t="inlineStr"/>
+      <c r="H1088" t="inlineStr">
+        <is>
+          <t>Regional HQ</t>
+        </is>
+      </c>
       <c r="I1088" t="inlineStr">
         <is>
           <t>IAP</t>
@@ -49389,7 +49413,11 @@
       <c r="G1089" t="n">
         <v>50040</v>
       </c>
-      <c r="H1089" t="inlineStr"/>
+      <c r="H1089" t="inlineStr">
+        <is>
+          <t>Agronomy, Grain/Feed</t>
+        </is>
+      </c>
       <c r="I1089" t="inlineStr">
         <is>
           <t>IAP</t>
@@ -49430,7 +49458,11 @@
       <c r="G1090" t="n">
         <v>50041</v>
       </c>
-      <c r="H1090" t="inlineStr"/>
+      <c r="H1090" t="inlineStr">
+        <is>
+          <t>Agronomy, Grain/Feed</t>
+        </is>
+      </c>
       <c r="I1090" t="inlineStr">
         <is>
           <t>IAP</t>
@@ -49471,7 +49503,11 @@
       <c r="G1091" t="n">
         <v>56014</v>
       </c>
-      <c r="H1091" t="inlineStr"/>
+      <c r="H1091" t="inlineStr">
+        <is>
+          <t>Grain/Feed</t>
+        </is>
+      </c>
       <c r="I1091" t="inlineStr">
         <is>
           <t>IAP</t>
@@ -49512,7 +49548,11 @@
       <c r="G1092" t="n">
         <v>50423</v>
       </c>
-      <c r="H1092" t="inlineStr"/>
+      <c r="H1092" t="inlineStr">
+        <is>
+          <t>Grain/Feed</t>
+        </is>
+      </c>
       <c r="I1092" t="inlineStr">
         <is>
           <t>IAP</t>
@@ -49553,7 +49593,11 @@
       <c r="G1093" t="n">
         <v>50006</v>
       </c>
-      <c r="H1093" t="inlineStr"/>
+      <c r="H1093" t="inlineStr">
+        <is>
+          <t>Agronomy</t>
+        </is>
+      </c>
       <c r="I1093" t="inlineStr">
         <is>
           <t>IAP</t>
@@ -49594,7 +49638,11 @@
       <c r="G1094" t="n">
         <v>50048</v>
       </c>
-      <c r="H1094" t="inlineStr"/>
+      <c r="H1094" t="inlineStr">
+        <is>
+          <t>Grain/Feed</t>
+        </is>
+      </c>
       <c r="I1094" t="inlineStr">
         <is>
           <t>IAP</t>
@@ -49635,7 +49683,11 @@
       <c r="G1095" t="n">
         <v>50050</v>
       </c>
-      <c r="H1095" t="inlineStr"/>
+      <c r="H1095" t="inlineStr">
+        <is>
+          <t>Grain/Feed</t>
+        </is>
+      </c>
       <c r="I1095" t="inlineStr">
         <is>
           <t>IAP</t>
@@ -49676,7 +49728,11 @@
       <c r="G1096" t="n">
         <v>50619</v>
       </c>
-      <c r="H1096" t="inlineStr"/>
+      <c r="H1096" t="inlineStr">
+        <is>
+          <t>Grain/Feed</t>
+        </is>
+      </c>
       <c r="I1096" t="inlineStr">
         <is>
           <t>IAP</t>
@@ -49717,7 +49773,11 @@
       <c r="G1097" t="n">
         <v>50055</v>
       </c>
-      <c r="H1097" t="inlineStr"/>
+      <c r="H1097" t="inlineStr">
+        <is>
+          <t>Agronomy</t>
+        </is>
+      </c>
       <c r="I1097" t="inlineStr">
         <is>
           <t>IAP</t>
@@ -49758,7 +49818,11 @@
       <c r="G1098" t="n">
         <v>50066</v>
       </c>
-      <c r="H1098" t="inlineStr"/>
+      <c r="H1098" t="inlineStr">
+        <is>
+          <t>Grain/Feed</t>
+        </is>
+      </c>
       <c r="I1098" t="inlineStr">
         <is>
           <t>IAP</t>
@@ -49799,7 +49863,11 @@
       <c r="G1099" t="n">
         <v>50309</v>
       </c>
-      <c r="H1099" t="inlineStr"/>
+      <c r="H1099" t="inlineStr">
+        <is>
+          <t>Agronomy, Grain/Feed</t>
+        </is>
+      </c>
       <c r="I1099" t="inlineStr">
         <is>
           <t>IAP</t>
@@ -49840,7 +49908,11 @@
       <c r="G1100" t="n">
         <v>50624</v>
       </c>
-      <c r="H1100" t="inlineStr"/>
+      <c r="H1100" t="inlineStr">
+        <is>
+          <t>Agronomy</t>
+        </is>
+      </c>
       <c r="I1100" t="inlineStr">
         <is>
           <t>IAP</t>
@@ -49881,7 +49953,11 @@
       <c r="G1101" t="n">
         <v>50535</v>
       </c>
-      <c r="H1101" t="inlineStr"/>
+      <c r="H1101" t="inlineStr">
+        <is>
+          <t>Agronomy, Grain/Feed</t>
+        </is>
+      </c>
       <c r="I1101" t="inlineStr">
         <is>
           <t>IAP</t>
@@ -49922,7 +49998,11 @@
       <c r="G1102" t="n">
         <v>50536</v>
       </c>
-      <c r="H1102" t="inlineStr"/>
+      <c r="H1102" t="inlineStr">
+        <is>
+          <t>Grain/Feed</t>
+        </is>
+      </c>
       <c r="I1102" t="inlineStr">
         <is>
           <t>IAP</t>
@@ -49963,7 +50043,11 @@
       <c r="G1103" t="n">
         <v>50538</v>
       </c>
-      <c r="H1103" t="inlineStr"/>
+      <c r="H1103" t="inlineStr">
+        <is>
+          <t>Agronomy, Grain/Feed</t>
+        </is>
+      </c>
       <c r="I1103" t="inlineStr">
         <is>
           <t>IAP</t>
@@ -50004,7 +50088,11 @@
       <c r="G1104" t="n">
         <v>50543</v>
       </c>
-      <c r="H1104" t="inlineStr"/>
+      <c r="H1104" t="inlineStr">
+        <is>
+          <t>Grain/Feed</t>
+        </is>
+      </c>
       <c r="I1104" t="inlineStr">
         <is>
           <t>IAP</t>
@@ -50045,7 +50133,11 @@
       <c r="G1105" t="n">
         <v>50543</v>
       </c>
-      <c r="H1105" t="inlineStr"/>
+      <c r="H1105" t="inlineStr">
+        <is>
+          <t>Agronomy</t>
+        </is>
+      </c>
       <c r="I1105" t="inlineStr">
         <is>
           <t>IAP</t>
@@ -50086,7 +50178,11 @@
       <c r="G1106" t="n">
         <v>50543</v>
       </c>
-      <c r="H1106" t="inlineStr"/>
+      <c r="H1106" t="inlineStr">
+        <is>
+          <t>Grain/Feed</t>
+        </is>
+      </c>
       <c r="I1106" t="inlineStr">
         <is>
           <t>IAP</t>
@@ -50127,7 +50223,11 @@
       <c r="G1107" t="n">
         <v>50636</v>
       </c>
-      <c r="H1107" t="inlineStr"/>
+      <c r="H1107" t="inlineStr">
+        <is>
+          <t>Grain/Feed</t>
+        </is>
+      </c>
       <c r="I1107" t="inlineStr">
         <is>
           <t>IAP</t>
@@ -50168,7 +50268,11 @@
       <c r="G1108" t="n">
         <v>50117</v>
       </c>
-      <c r="H1108" t="inlineStr"/>
+      <c r="H1108" t="inlineStr">
+        <is>
+          <t>Grain/Feed</t>
+        </is>
+      </c>
       <c r="I1108" t="inlineStr">
         <is>
           <t>IAP</t>
@@ -50209,7 +50313,11 @@
       <c r="G1109" t="n">
         <v>51445</v>
       </c>
-      <c r="H1109" t="inlineStr"/>
+      <c r="H1109" t="inlineStr">
+        <is>
+          <t>Grain/Feed</t>
+        </is>
+      </c>
       <c r="I1109" t="inlineStr">
         <is>
           <t>IAP</t>
@@ -50250,7 +50358,11 @@
       <c r="G1110" t="n">
         <v>50129</v>
       </c>
-      <c r="H1110" t="inlineStr"/>
+      <c r="H1110" t="inlineStr">
+        <is>
+          <t>Agronomy</t>
+        </is>
+      </c>
       <c r="I1110" t="inlineStr">
         <is>
           <t>IAP</t>
@@ -50291,7 +50403,11 @@
       <c r="G1111" t="n">
         <v>50129</v>
       </c>
-      <c r="H1111" t="inlineStr"/>
+      <c r="H1111" t="inlineStr">
+        <is>
+          <t>Agronomy</t>
+        </is>
+      </c>
       <c r="I1111" t="inlineStr">
         <is>
           <t>IAP</t>
@@ -50332,7 +50448,11 @@
       <c r="G1112" t="n">
         <v>51449</v>
       </c>
-      <c r="H1112" t="inlineStr"/>
+      <c r="H1112" t="inlineStr">
+        <is>
+          <t>Grain/Feed</t>
+        </is>
+      </c>
       <c r="I1112" t="inlineStr">
         <is>
           <t>IAP</t>
@@ -50373,7 +50493,11 @@
       <c r="G1113" t="n">
         <v>51450</v>
       </c>
-      <c r="H1113" t="inlineStr"/>
+      <c r="H1113" t="inlineStr">
+        <is>
+          <t>Grain/Feed</t>
+        </is>
+      </c>
       <c r="I1113" t="inlineStr">
         <is>
           <t>IAP</t>
@@ -50414,7 +50538,11 @@
       <c r="G1114" t="n">
         <v>50452</v>
       </c>
-      <c r="H1114" t="inlineStr"/>
+      <c r="H1114" t="inlineStr">
+        <is>
+          <t>Grain/Feed</t>
+        </is>
+      </c>
       <c r="I1114" t="inlineStr">
         <is>
           <t>IAP</t>
@@ -50455,7 +50583,11 @@
       <c r="G1115" t="n">
         <v>51454</v>
       </c>
-      <c r="H1115" t="inlineStr"/>
+      <c r="H1115" t="inlineStr">
+        <is>
+          <t>Grain/Feed</t>
+        </is>
+      </c>
       <c r="I1115" t="inlineStr">
         <is>
           <t>IAP</t>
@@ -50496,7 +50628,11 @@
       <c r="G1116" t="n">
         <v>62859</v>
       </c>
-      <c r="H1116" t="inlineStr"/>
+      <c r="H1116" t="inlineStr">
+        <is>
+          <t>Grain/Feed</t>
+        </is>
+      </c>
       <c r="I1116" t="inlineStr">
         <is>
           <t>IAP</t>
@@ -50537,7 +50673,11 @@
       <c r="G1117" t="n">
         <v>50169</v>
       </c>
-      <c r="H1117" t="inlineStr"/>
+      <c r="H1117" t="inlineStr">
+        <is>
+          <t>Grain/Feed</t>
+        </is>
+      </c>
       <c r="I1117" t="inlineStr">
         <is>
           <t>IAP</t>
@@ -50578,7 +50718,11 @@
       <c r="G1118" t="n">
         <v>50660</v>
       </c>
-      <c r="H1118" t="inlineStr"/>
+      <c r="H1118" t="inlineStr">
+        <is>
+          <t>Grain/Feed</t>
+        </is>
+      </c>
       <c r="I1118" t="inlineStr">
         <is>
           <t>IAP</t>
@@ -50619,7 +50763,11 @@
       <c r="G1119" t="n">
         <v>50568</v>
       </c>
-      <c r="H1119" t="inlineStr"/>
+      <c r="H1119" t="inlineStr">
+        <is>
+          <t>Grain/Feed</t>
+        </is>
+      </c>
       <c r="I1119" t="inlineStr">
         <is>
           <t>IAP</t>
@@ -50660,7 +50808,11 @@
       <c r="G1120" t="n">
         <v>51458</v>
       </c>
-      <c r="H1120" t="inlineStr"/>
+      <c r="H1120" t="inlineStr">
+        <is>
+          <t>Grain/Feed</t>
+        </is>
+      </c>
       <c r="I1120" t="inlineStr">
         <is>
           <t>IAP</t>
@@ -50701,7 +50853,11 @@
       <c r="G1121" t="n">
         <v>50216</v>
       </c>
-      <c r="H1121" t="inlineStr"/>
+      <c r="H1121" t="inlineStr">
+        <is>
+          <t>Grain/Feed</t>
+        </is>
+      </c>
       <c r="I1121" t="inlineStr">
         <is>
           <t>IAP</t>
@@ -50742,7 +50898,11 @@
       <c r="G1122" t="n">
         <v>50217</v>
       </c>
-      <c r="H1122" t="inlineStr"/>
+      <c r="H1122" t="inlineStr">
+        <is>
+          <t>Grain/Feed</t>
+        </is>
+      </c>
       <c r="I1122" t="inlineStr">
         <is>
           <t>IAP</t>
@@ -50783,7 +50943,11 @@
       <c r="G1123" t="n">
         <v>50220</v>
       </c>
-      <c r="H1123" t="inlineStr"/>
+      <c r="H1123" t="inlineStr">
+        <is>
+          <t>Agronomy, Grain/Feed</t>
+        </is>
+      </c>
       <c r="I1123" t="inlineStr">
         <is>
           <t>IAP</t>
@@ -50824,7 +50988,11 @@
       <c r="G1124" t="n">
         <v>50327</v>
       </c>
-      <c r="H1124" t="inlineStr"/>
+      <c r="H1124" t="inlineStr">
+        <is>
+          <t>Grain/Feed</t>
+        </is>
+      </c>
       <c r="I1124" t="inlineStr">
         <is>
           <t>IAP</t>
@@ -50865,7 +51033,11 @@
       <c r="G1125" t="n">
         <v>50465</v>
       </c>
-      <c r="H1125" t="inlineStr"/>
+      <c r="H1125" t="inlineStr">
+        <is>
+          <t>Agronomy, Grain/Feed</t>
+        </is>
+      </c>
       <c r="I1125" t="inlineStr">
         <is>
           <t>IAP</t>
@@ -50906,7 +51078,11 @@
       <c r="G1126" t="n">
         <v>51459</v>
       </c>
-      <c r="H1126" t="inlineStr"/>
+      <c r="H1126" t="inlineStr">
+        <is>
+          <t>Grain/Feed</t>
+        </is>
+      </c>
       <c r="I1126" t="inlineStr">
         <is>
           <t>IAP</t>
@@ -50947,7 +51123,11 @@
       <c r="G1127" t="n">
         <v>50235</v>
       </c>
-      <c r="H1127" t="inlineStr"/>
+      <c r="H1127" t="inlineStr">
+        <is>
+          <t>Grain/Feed</t>
+        </is>
+      </c>
       <c r="I1127" t="inlineStr">
         <is>
           <t>IAP</t>
@@ -50988,7 +51168,11 @@
       <c r="G1128" t="n">
         <v>50579</v>
       </c>
-      <c r="H1128" t="inlineStr"/>
+      <c r="H1128" t="inlineStr">
+        <is>
+          <t>Grain/Feed</t>
+        </is>
+      </c>
       <c r="I1128" t="inlineStr">
         <is>
           <t>IAP</t>
@@ -51029,7 +51213,11 @@
       <c r="G1129" t="n">
         <v>46173</v>
       </c>
-      <c r="H1129" t="inlineStr"/>
+      <c r="H1129" t="inlineStr">
+        <is>
+          <t>Grain/Feed</t>
+        </is>
+      </c>
       <c r="I1129" t="inlineStr">
         <is>
           <t>IAP</t>
@@ -51070,7 +51258,11 @@
       <c r="G1130" t="n">
         <v>50586</v>
       </c>
-      <c r="H1130" t="inlineStr"/>
+      <c r="H1130" t="inlineStr">
+        <is>
+          <t>Grain/Feed</t>
+        </is>
+      </c>
       <c r="I1130" t="inlineStr">
         <is>
           <t>IAP</t>
@@ -51111,7 +51303,11 @@
       <c r="G1131" t="n">
         <v>50588</v>
       </c>
-      <c r="H1131" t="inlineStr"/>
+      <c r="H1131" t="inlineStr">
+        <is>
+          <t>Grain/Feed</t>
+        </is>
+      </c>
       <c r="I1131" t="inlineStr">
         <is>
           <t>IAP</t>
@@ -51152,7 +51348,11 @@
       <c r="G1132" t="n">
         <v>51463</v>
       </c>
-      <c r="H1132" t="inlineStr"/>
+      <c r="H1132" t="inlineStr">
+        <is>
+          <t>Agronomy, Grain/Feed</t>
+        </is>
+      </c>
       <c r="I1132" t="inlineStr">
         <is>
           <t>IAP</t>
@@ -51193,7 +51393,11 @@
       <c r="G1133" t="n">
         <v>50677</v>
       </c>
-      <c r="H1133" t="inlineStr"/>
+      <c r="H1133" t="inlineStr">
+        <is>
+          <t>Grain/Feed</t>
+        </is>
+      </c>
       <c r="I1133" t="inlineStr">
         <is>
           <t>IAP</t>
@@ -51234,7 +51438,11 @@
       <c r="G1134" t="n">
         <v>50680</v>
       </c>
-      <c r="H1134" t="inlineStr"/>
+      <c r="H1134" t="inlineStr">
+        <is>
+          <t>Grain/Feed</t>
+        </is>
+      </c>
       <c r="I1134" t="inlineStr">
         <is>
           <t>IAP</t>
@@ -51275,7 +51483,11 @@
       <c r="G1135" t="n">
         <v>50277</v>
       </c>
-      <c r="H1135" t="inlineStr"/>
+      <c r="H1135" t="inlineStr">
+        <is>
+          <t>Grain/Feed</t>
+        </is>
+      </c>
       <c r="I1135" t="inlineStr">
         <is>
           <t>IAP</t>
@@ -51316,7 +51528,11 @@
       <c r="G1136" t="n">
         <v>51433</v>
       </c>
-      <c r="H1136" t="inlineStr"/>
+      <c r="H1136" t="inlineStr">
+        <is>
+          <t>Agronomy, Grain/Feed</t>
+        </is>
+      </c>
       <c r="I1136" t="inlineStr">
         <is>
           <t>IAP</t>
@@ -56372,7 +56588,7 @@
       </c>
       <c r="C1249" t="inlineStr">
         <is>
-          <t xml:space="preserve">Wellsburg </t>
+          <t>Wellsburg</t>
         </is>
       </c>
       <c r="D1249" t="inlineStr">

</xml_diff>